<commit_message>
update cetak laporan deviasi
</commit_message>
<xml_diff>
--- a/storage/template/laporan-deviasi.xlsx
+++ b/storage/template/laporan-deviasi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\biroap2\storage\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F88339D-DCE9-4EF0-884E-5146BCB2C308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A99B12-9957-42BB-897D-BCA102310637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EDE6994B-93EA-4551-88D6-2B1820C54DC1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>No.</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Deviasi</t>
+  </si>
+  <si>
+    <t>SERAPAN KEUANGAN APBD PER OPD SAMPAI DENGAN FEBRUARI 2023</t>
+  </si>
+  <si>
+    <t>PEMERINTAH PROVINSI NUSA TENGGARA BARAT</t>
   </si>
 </sst>
 </file>
@@ -97,7 +103,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -146,11 +152,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +174,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -475,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182553DD-7CE7-4E1E-AE3C-93931E5D44A7}">
-  <dimension ref="A3:I4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -483,6 +504,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
@@ -528,9 +575,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>